<commit_message>
#4 makes me want to die
</commit_message>
<xml_diff>
--- a/Copy of Members.xlsx
+++ b/Copy of Members.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="2580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="2580" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OldMembers" sheetId="1" r:id="rId1"/>
@@ -1025,7 +1025,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1832,7 +1832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="A2:D17"/>
     </sheetView>
   </sheetViews>
@@ -2127,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>